<commit_message>
creating another branch from admin-manage
</commit_message>
<xml_diff>
--- a/src/main/resources/Data.xlsx
+++ b/src/main/resources/Data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbhattacharjee\Desktop\CrossSkillingAutomation\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF1D53E-EE0B-47F3-B3AC-017BBF4FF454}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,12 +24,85 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>email id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work ex </t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>tb_0</t>
+  </si>
+  <si>
+    <t>tb@g.com</t>
+  </si>
+  <si>
+    <t>sdet</t>
+  </si>
+  <si>
+    <t>coder</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>tb_1</t>
+  </si>
+  <si>
+    <t>tb_2</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>React.js, Angular</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +125,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +412,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C56B1722-DF3C-486D-802B-3BD0ACA73632}"/>
+    <hyperlink ref="B3:B4" r:id="rId2" display="tb@g.com" xr:uid="{7255DAAE-74E8-45BB-8358-5AD92D156021}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>